<commit_message>
feat(table category): Added both migration and model for the category table
</commit_message>
<xml_diff>
--- a/doc/routes-a-faire.xlsx
+++ b/doc/routes-a-faire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ps46bhd\Desktop\github\P_Web-295\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C532E418-E5DB-4F8D-A6D3-1F9FF4E86117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8127BF-4809-4AE2-A125-6312DEB17F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,15 +200,6 @@
     <t>OBLIGATOIRE</t>
   </si>
   <si>
-    <t>/writer</t>
-  </si>
-  <si>
-    <t>/writer/id</t>
-  </si>
-  <si>
-    <t>writer</t>
-  </si>
-  <si>
     <t>/books?limit=5</t>
   </si>
   <si>
@@ -234,6 +225,15 @@
   </si>
   <si>
     <t>username, password</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>/author</t>
+  </si>
+  <si>
+    <t>/author/id</t>
   </si>
 </sst>
 </file>
@@ -586,7 +586,7 @@
   <dimension ref="B2:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +626,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
         <v>20</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -699,7 +699,7 @@
         <v>19</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -726,7 +726,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>21</v>
@@ -767,7 +767,7 @@
         <v>20</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -833,7 +833,7 @@
         <v>20</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
@@ -868,7 +868,7 @@
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>9</v>
@@ -877,7 +877,7 @@
         <v>3</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>20</v>
@@ -896,13 +896,13 @@
         <v>4</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>20</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="2"/>
@@ -918,7 +918,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>41</v>
@@ -937,7 +937,7 @@
         <v>6</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>41</v>
@@ -979,7 +979,7 @@
         <v>20</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
@@ -1049,7 +1049,7 @@
         <v>14</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>43</v>
@@ -1100,7 +1100,7 @@
         <v>21</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat(route): added all routes and controller in route.ts
</commit_message>
<xml_diff>
--- a/doc/routes-a-faire.xlsx
+++ b/doc/routes-a-faire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ps46bhd\Desktop\github\P_Web-295\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8127BF-4809-4AE2-A125-6312DEB17F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42003C32-DB00-46D2-8394-44B44E7A03E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="67">
   <si>
     <t>ROUTES</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>/author/id</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -583,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S40"/>
+  <dimension ref="A2:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +604,7 @@
     <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>53</v>
       </c>
@@ -609,7 +612,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -629,10 +632,13 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -650,7 +656,10 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
       <c r="B6" s="1"/>
       <c r="C6" s="6" t="s">
         <v>10</v>
@@ -666,7 +675,10 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="6" t="s">
         <v>12</v>
@@ -684,7 +696,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="6" t="s">
         <v>11</v>
@@ -702,7 +717,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="6" t="s">
         <v>13</v>
@@ -718,7 +736,7 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="s">
         <v>24</v>
       </c>
@@ -732,10 +750,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
       <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
@@ -753,7 +774,10 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
       <c r="C13" s="6" t="s">
         <v>25</v>
       </c>
@@ -770,7 +794,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
       <c r="C14" s="7" t="s">
         <v>11</v>
       </c>
@@ -784,7 +811,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
       <c r="C15" s="7" t="s">
         <v>13</v>
       </c>
@@ -798,10 +828,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
       <c r="B17" s="4" t="s">
         <v>27</v>
       </c>
@@ -819,7 +852,10 @@
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
       <c r="C18" s="6" t="s">
         <v>12</v>
       </c>
@@ -836,7 +872,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
       <c r="C19" s="9" t="s">
         <v>11</v>
       </c>
@@ -855,7 +894,7 @@
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -866,7 +905,10 @@
       <c r="R20" s="1"/>
       <c r="S20" s="2"/>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
       <c r="B21" s="4" t="s">
         <v>63</v>
       </c>
@@ -888,7 +930,10 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
       <c r="C22" s="6" t="s">
         <v>12</v>
       </c>
@@ -910,7 +955,10 @@
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
       <c r="C23" s="9" t="s">
         <v>11</v>
       </c>
@@ -929,7 +977,10 @@
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
       <c r="C24" s="9" t="s">
         <v>13</v>
       </c>
@@ -948,7 +999,10 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
       <c r="B26" s="4" t="s">
         <v>15</v>
       </c>
@@ -965,7 +1019,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
       <c r="C27" s="12" t="s">
         <v>12</v>
       </c>
@@ -982,7 +1039,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
       <c r="C28" s="6" t="s">
         <v>44</v>
       </c>
@@ -996,7 +1056,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>66</v>
+      </c>
       <c r="C29" s="8" t="s">
         <v>11</v>
       </c>
@@ -1010,7 +1073,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
       <c r="C30" s="8" t="s">
         <v>13</v>
       </c>
@@ -1024,7 +1090,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
       <c r="B32" s="4" t="s">
         <v>20</v>
       </c>
@@ -1041,7 +1110,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
       <c r="C33" s="6" t="s">
         <v>42</v>
       </c>
@@ -1055,7 +1127,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
       <c r="C34" s="9" t="s">
         <v>39</v>
       </c>
@@ -1069,7 +1144,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
       <c r="C35" s="9" t="s">
         <v>9</v>
       </c>
@@ -1083,7 +1161,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>66</v>
+      </c>
       <c r="B38" s="4" t="s">
         <v>30</v>
       </c>
@@ -1103,7 +1184,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>66</v>
+      </c>
       <c r="C39" s="6" t="s">
         <v>35</v>
       </c>
@@ -1117,7 +1201,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>66</v>
+      </c>
       <c r="C40" s="9" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
feat(authorController): Added 2 controls to get all authors and add one author
</commit_message>
<xml_diff>
--- a/doc/routes-a-faire.xlsx
+++ b/doc/routes-a-faire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ps46bhd\Desktop\github\P_Web-295\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42003C32-DB00-46D2-8394-44B44E7A03E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCE7E5E-2009-431A-9D85-F62C3F370570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="66">
   <si>
     <t>ROUTES</t>
   </si>
@@ -234,9 +234,6 @@
   </si>
   <si>
     <t>/author/id</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -586,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:S40"/>
+  <dimension ref="B2:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +601,7 @@
     <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>53</v>
       </c>
@@ -612,7 +609,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -632,13 +629,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>66</v>
-      </c>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -656,10 +650,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>66</v>
-      </c>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="6" t="s">
         <v>10</v>
@@ -675,10 +666,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>66</v>
-      </c>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="6" t="s">
         <v>12</v>
@@ -696,10 +684,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>66</v>
-      </c>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="6" t="s">
         <v>11</v>
@@ -717,10 +702,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>66</v>
-      </c>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="6" t="s">
         <v>13</v>
@@ -736,7 +718,7 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="s">
         <v>24</v>
       </c>
@@ -750,13 +732,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>66</v>
-      </c>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
@@ -774,10 +753,7 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>66</v>
-      </c>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>25</v>
       </c>
@@ -794,10 +770,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>66</v>
-      </c>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C14" s="7" t="s">
         <v>11</v>
       </c>
@@ -811,10 +784,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>66</v>
-      </c>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C15" s="7" t="s">
         <v>13</v>
       </c>
@@ -828,13 +798,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>66</v>
-      </c>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>27</v>
       </c>
@@ -852,10 +819,7 @@
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>66</v>
-      </c>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C18" s="6" t="s">
         <v>12</v>
       </c>
@@ -872,10 +836,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>66</v>
-      </c>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C19" s="9" t="s">
         <v>11</v>
       </c>
@@ -894,7 +855,7 @@
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -905,10 +866,7 @@
       <c r="R20" s="1"/>
       <c r="S20" s="2"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>66</v>
-      </c>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>63</v>
       </c>
@@ -930,10 +888,7 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>66</v>
-      </c>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C22" s="6" t="s">
         <v>12</v>
       </c>
@@ -955,10 +910,7 @@
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>66</v>
-      </c>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C23" s="9" t="s">
         <v>11</v>
       </c>
@@ -977,10 +929,7 @@
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>66</v>
-      </c>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C24" s="9" t="s">
         <v>13</v>
       </c>
@@ -999,10 +948,7 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>66</v>
-      </c>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>15</v>
       </c>
@@ -1019,10 +965,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>66</v>
-      </c>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C27" s="12" t="s">
         <v>12</v>
       </c>
@@ -1039,10 +982,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>66</v>
-      </c>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C28" s="6" t="s">
         <v>44</v>
       </c>
@@ -1056,10 +996,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>66</v>
-      </c>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C29" s="8" t="s">
         <v>11</v>
       </c>
@@ -1073,10 +1010,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>66</v>
-      </c>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C30" s="8" t="s">
         <v>13</v>
       </c>
@@ -1090,10 +1024,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>66</v>
-      </c>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>20</v>
       </c>
@@ -1110,10 +1041,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>66</v>
-      </c>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C33" s="6" t="s">
         <v>42</v>
       </c>
@@ -1127,10 +1055,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>66</v>
-      </c>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C34" s="9" t="s">
         <v>39</v>
       </c>
@@ -1144,10 +1069,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>66</v>
-      </c>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C35" s="9" t="s">
         <v>9</v>
       </c>
@@ -1161,10 +1083,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>66</v>
-      </c>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
         <v>30</v>
       </c>
@@ -1184,10 +1103,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>66</v>
-      </c>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C39" s="6" t="s">
         <v>35</v>
       </c>
@@ -1201,10 +1117,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>66</v>
-      </c>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C40" s="9" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
chore(rapport): ajout du rapport au depot
</commit_message>
<xml_diff>
--- a/doc/routes-a-faire.xlsx
+++ b/doc/routes-a-faire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ps46bhd\Desktop\github\P_Web-295\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B43ED14-1266-4D29-9C6E-3D64AFE1D8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC2CFE0-F7FE-4116-9CA5-C8B196EB358D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="7200" yWindow="3750" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>